<commit_message>
4.11 - updates to Compatibility
</commit_message>
<xml_diff>
--- a/Muhurtha.Core/data/PeopleList.xlsx
+++ b/Muhurtha.Core/data/PeopleList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="39">
   <si>
     <t>Name</t>
   </si>
@@ -129,6 +129,18 @@
   </si>
   <si>
     <t>Klang</t>
+  </si>
+  <si>
+    <t>Rubeshen</t>
+  </si>
+  <si>
+    <t>23:35 15/05/1992 +08:00</t>
+  </si>
+  <si>
+    <t>Haravin</t>
+  </si>
+  <si>
+    <t>04:10 25/03/1991 +08:00</t>
   </si>
 </sst>
 </file>
@@ -224,8 +236,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F12" tableType="xml" totalsRowShown="0" connectionId="1">
-  <autoFilter ref="A1:F12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F14" tableType="xml" totalsRowShown="0" connectionId="1">
+  <autoFilter ref="A1:F14"/>
   <tableColumns count="6">
     <tableColumn id="1" uniqueName="Name" name="Name">
       <xmlColumnPr mapId="1" xpath="/Root/Person/Name" xmlDataType="string"/>
@@ -537,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,6 +805,46 @@
         <v>30</v>
       </c>
     </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13">
+        <v>101.4456</v>
+      </c>
+      <c r="E13">
+        <v>3.0449000000000002</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14">
+        <v>101.68729999999999</v>
+      </c>
+      <c r="E14">
+        <v>3.1602700000000001</v>
+      </c>
+      <c r="F14" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>